<commit_message>
unitest crane load and unload and visual test
</commit_message>
<xml_diff>
--- a/CodeVS/data/input/Tugboat Problem V5-Demo.xlsx
+++ b/CodeVS/data/input/Tugboat Problem V5-Demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\Aj Kanchana Projects\TugBoat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\Aj Kanchana Projects\Tugboat\CodeVS\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5095F59D-1CF9-4965-AFC2-796C0556FC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED19926-1D8E-4527-B1D5-F3A3BCB7FF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="251">
   <si>
     <t>ID</t>
   </si>
@@ -1215,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -3627,8 +3627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4594,7 +4594,9 @@
       <c r="G30" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="30"/>
+      <c r="H30" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="J30" s="29">
         <v>20</v>
       </c>
@@ -4624,7 +4626,9 @@
       <c r="G31" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="30"/>
+      <c r="H31" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="J31" s="29">
         <v>20</v>
       </c>
@@ -4984,7 +4988,9 @@
       <c r="G42" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="36"/>
+      <c r="H42" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I42" s="33"/>
       <c r="J42" s="35">
         <v>20</v>
@@ -5015,7 +5021,9 @@
       <c r="G43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I43" s="3"/>
       <c r="J43" s="5">
         <v>20</v>
@@ -5046,7 +5054,9 @@
       <c r="G44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="6"/>
+      <c r="H44" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="J44" s="5">
         <v>20</v>
@@ -5077,7 +5087,9 @@
       <c r="G45" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H45" s="6"/>
+      <c r="H45" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I45" s="3"/>
       <c r="J45" s="5">
         <v>20</v>
@@ -5108,7 +5120,9 @@
       <c r="G46" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H46" s="6"/>
+      <c r="H46" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I46" s="3"/>
       <c r="J46" s="5">
         <v>20</v>
@@ -5139,7 +5153,9 @@
       <c r="G47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H47" s="6"/>
+      <c r="H47" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I47" s="3"/>
       <c r="J47" s="5">
         <v>20</v>
@@ -5170,7 +5186,9 @@
       <c r="G48" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H48" s="6"/>
+      <c r="H48" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I48" s="3"/>
       <c r="J48" s="5">
         <v>20</v>
@@ -5201,7 +5219,9 @@
       <c r="G49" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H49" s="6"/>
+      <c r="H49" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I49" s="3"/>
       <c r="J49" s="5">
         <v>20</v>
@@ -5232,7 +5252,9 @@
       <c r="G50" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H50" s="6"/>
+      <c r="H50" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I50" s="3"/>
       <c r="J50" s="5">
         <v>20</v>
@@ -5263,7 +5285,9 @@
       <c r="G51" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H51" s="6"/>
+      <c r="H51" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="I51" s="3"/>
       <c r="J51" s="5">
         <v>20</v>

</xml_diff>

<commit_message>
emtry time compute step move detail
</commit_message>
<xml_diff>
--- a/CodeVS/data/input/Tugboat Problem V5-Demo.xlsx
+++ b/CodeVS/data/input/Tugboat Problem V5-Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\Aj Kanchana Projects\Tugboat\CodeVS\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED19926-1D8E-4527-B1D5-F3A3BCB7FF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7ADBE5-DEBC-44E8-8C69-3A6D8ACD7FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="5" r:id="rId1"/>
@@ -1216,7 +1216,7 @@
   <dimension ref="A1:W993"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3627,16 +3627,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42:H51"/>
+    <sheetView topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F42" activeCellId="1" sqref="E42 F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="5" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" customWidth="1"/>
@@ -6576,8 +6575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O1003"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8449,8 +8448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8495,11 +8494,11 @@
       <c r="C2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="1">
-        <v>13.183107989899099</v>
-      </c>
-      <c r="E2" s="1">
-        <v>100.812638437557</v>
+      <c r="D2" s="35">
+        <v>13.188484284522699</v>
+      </c>
+      <c r="E2" s="35">
+        <v>100.81514283237</v>
       </c>
       <c r="F2" s="1">
         <v>39</v>

</xml_diff>